<commit_message>
completed hand calculations and table for results
</commit_message>
<xml_diff>
--- a/MOSFET/Data/proj1.xlsx
+++ b/MOSFET/Data/proj1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\3131\Projects\MOSFET\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C497B29-91DD-4226-ABE2-B0FE6F1992FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27FD10C-07E9-4F81-BBF1-3E98B7EB7471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{412FF896-E87B-462B-A573-5628840FFF8E}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{412FF896-E87B-462B-A573-5628840FFF8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>VDS</t>
   </si>
@@ -132,6 +132,33 @@
   </si>
   <si>
     <t>3dB 2</t>
+  </si>
+  <si>
+    <t>Theoretical</t>
+  </si>
+  <si>
+    <t>Simulated</t>
+  </si>
+  <si>
+    <t>ID (uA)</t>
+  </si>
+  <si>
+    <t>Experimental</t>
+  </si>
+  <si>
+    <t>VGS (V)</t>
+  </si>
+  <si>
+    <t>VDS (V)</t>
+  </si>
+  <si>
+    <t>Gain (V/V)</t>
+  </si>
+  <si>
+    <t>Rin (KOHM)</t>
+  </si>
+  <si>
+    <t>Rout (KOHM)</t>
   </si>
 </sst>
 </file>
@@ -483,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93600F92-4588-4B96-A9C6-A8A79A2E880B}">
-  <dimension ref="A2:G35"/>
+  <dimension ref="A2:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,10 +523,13 @@
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -519,7 +549,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>60</v>
       </c>
@@ -534,11 +564,20 @@
         <v>34.199999999999996</v>
       </c>
       <c r="E3">
-        <f>20*LOG10(D3)</f>
+        <f t="shared" ref="E3:E10" si="0">20*LOG10(D3)</f>
         <v>30.680522121122699</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>15000</v>
       </c>
@@ -549,15 +588,27 @@
         <v>3.6</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D15" si="0">C4/B4</f>
+        <f t="shared" ref="D4:D15" si="1">C4/B4</f>
         <v>36</v>
       </c>
       <c r="E4">
-        <f>20*LOG10(D4)</f>
+        <f t="shared" si="0"/>
         <v>31.126050015345747</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4">
+        <v>2.3570000000000002</v>
+      </c>
+      <c r="K4">
+        <v>2.3570000000000002</v>
+      </c>
+      <c r="L4">
+        <v>2.423</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>22000</v>
       </c>
@@ -568,15 +619,27 @@
         <v>3.6</v>
       </c>
       <c r="D5">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="E5">
         <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="E5">
-        <f>20*LOG10(D5)</f>
         <v>31.126050015345747</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5">
+        <v>6.7830000000000004</v>
+      </c>
+      <c r="K5">
+        <v>6.7839999999999998</v>
+      </c>
+      <c r="L5">
+        <v>6.8730000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>23000</v>
       </c>
@@ -587,15 +650,27 @@
         <v>3.58</v>
       </c>
       <c r="D6">
+        <f t="shared" si="1"/>
+        <v>35.799999999999997</v>
+      </c>
+      <c r="E6">
         <f t="shared" si="0"/>
-        <v>35.799999999999997</v>
-      </c>
-      <c r="E6">
-        <f>20*LOG10(D6)</f>
         <v>31.077660532877488</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6">
+        <v>678</v>
+      </c>
+      <c r="K6">
+        <v>678</v>
+      </c>
+      <c r="L6">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>600</v>
       </c>
@@ -606,15 +681,27 @@
         <v>3.46</v>
       </c>
       <c r="D7">
+        <f t="shared" si="1"/>
+        <v>34.599999999999994</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="0"/>
-        <v>34.599999999999994</v>
-      </c>
-      <c r="E7">
-        <f>20*LOG10(D7)</f>
         <v>30.781521975855529</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7">
+        <v>69.774000000000001</v>
+      </c>
+      <c r="K7">
+        <v>68.91</v>
+      </c>
+      <c r="L7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>226000</v>
       </c>
@@ -625,15 +712,27 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="D8">
+        <f t="shared" si="1"/>
+        <v>25.499999999999996</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="0"/>
-        <v>25.499999999999996</v>
-      </c>
-      <c r="E8">
-        <f>20*LOG10(D8)</f>
         <v>28.130803608679102</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8">
+        <v>7.1050000000000004</v>
+      </c>
+      <c r="K8">
+        <v>7.11</v>
+      </c>
+      <c r="L8">
+        <v>7.194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>24</v>
       </c>
@@ -644,15 +743,27 @@
         <v>2.548</v>
       </c>
       <c r="D9">
+        <f t="shared" si="1"/>
+        <v>25.48</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="0"/>
-        <v>25.48</v>
-      </c>
-      <c r="E9">
-        <f>20*LOG10(D9)</f>
         <v>28.123988473266259</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9">
+        <v>6.2069999999999999</v>
+      </c>
+      <c r="K9">
+        <v>6.2110000000000003</v>
+      </c>
+      <c r="L9">
+        <v>6.3289999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>400</v>
       </c>
@@ -663,15 +774,15 @@
         <v>3.6</v>
       </c>
       <c r="D10">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="E10">
-        <f>20*LOG10(D10)</f>
         <v>31.126050015345747</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>22</v>
       </c>
@@ -682,7 +793,7 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25.499999999999996</v>
       </c>
       <c r="E12">
@@ -693,7 +804,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>300</v>
       </c>
@@ -704,7 +815,7 @@
         <v>3.6</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="E13">
@@ -715,7 +826,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>25000</v>
       </c>
@@ -726,7 +837,7 @@
         <v>3.6</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="E14">
@@ -737,7 +848,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>915000</v>
       </c>
@@ -748,7 +859,7 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25.499999999999996</v>
       </c>
       <c r="E15">

</xml_diff>

<commit_message>
added simulated data for BJT
</commit_message>
<xml_diff>
--- a/MOSFET/Data/proj1.xlsx
+++ b/MOSFET/Data/proj1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\3131\Projects\MOSFET\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27FD10C-07E9-4F81-BBF1-3E98B7EB7471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D8DE97-9632-4D28-B412-C9DA3A5314CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{412FF896-E87B-462B-A573-5628840FFF8E}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{412FF896-E87B-462B-A573-5628840FFF8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
   <dimension ref="A2:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>